<commit_message>
Ny mal for tariffendring excel ark
</commit_message>
<xml_diff>
--- a/src/test/resources/koronasykepengerefusjon_tariffendringer_nav_TESTFILE.xlsx
+++ b/src/test/resources/koronasykepengerefusjon_tariffendringer_nav_TESTFILE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustav/projects/sporenstreks/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7776CB14-772F-4643-96DB-EA229956DE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880559A8-5270-9342-AFC7-47A7491F08B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35840" yWindow="500" windowWidth="51200" windowHeight="26600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,13 +99,13 @@
     <t>16.03.2020</t>
   </si>
   <si>
-    <t>Utvidet refusjon av sykepenger i forbindelse med koronaviruset - tariffendringer</t>
+    <t xml:space="preserve">Du kan max legge til 5000 arbeidstakere. Er ikke dette tilstrekkelig, må du fylle ut og laste opp i flere omganger. </t>
   </si>
   <si>
-    <t xml:space="preserve">Dette dokumentet er beregnet på virksomheter som har sendt krav tidligere, men som på bakgrunn av tarffendringer ønsker å sende et oppdatert krav. Legg inn ny totalbeløp, så beregner NAV differansen mellom gammelt og nytt krav.  </t>
+    <t xml:space="preserve">Dette dokumentet er beregnet på virksomheter som har sendt krav tidligere, men som på bakgrunn av f.eks. tariffendringer ønsker å sende et oppdatert krav. Legg inn ny totalbeløp, så beregner NAV differansen mellom gammelt og nytt krav.  </t>
   </si>
   <si>
-    <t xml:space="preserve">Du kan max legge til 5000 arbeidstakere. Er ikke dette tilstrekkelig, må du fylle ut og laste opp i flere omganger. </t>
+    <t>Utvidet refusjon av sykepenger i forbindelse med koronaviruset - endring av krav ved f.eks. tariffendringer</t>
   </si>
 </sst>
 </file>
@@ -635,7 +635,7 @@
   <dimension ref="A1:Q1021"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,7 +650,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="37" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B1" s="14"/>
       <c r="F1" s="1"/>
@@ -676,13 +676,13 @@
       <c r="L3" s="19"/>
       <c r="M3" s="19"/>
       <c r="N3" s="19"/>
-      <c r="O3" s="8"/>
+      <c r="O3" s="19"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
     </row>
     <row r="4" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="17"/>

</xml_diff>